<commit_message>
Data type definitions added
Signed-off-by: UweSteinkeFromSiemens <uwe.steinke@siemens.com>
</commit_message>
<xml_diff>
--- a/System Analysis/SUBSET_26_3-6/Spread-sheet-SUBSET_26-2-6_Train-Position-Information.xlsx
+++ b/System Analysis/SUBSET_26_3-6/Spread-sheet-SUBSET_26-2-6_Train-Position-Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="101">
   <si>
     <t>Template for System Analysis</t>
   </si>
@@ -150,19 +150,10 @@
     <t>Floating point</t>
   </si>
   <si>
-    <t>textual description</t>
-  </si>
-  <si>
     <t>T_ident</t>
   </si>
   <si>
-    <t>based on a textual  description</t>
-  </si>
-  <si>
     <t xml:space="preserve">T_Version </t>
-  </si>
-  <si>
-    <t>{3.0.0, 3.3.0}</t>
   </si>
   <si>
     <r>
@@ -185,9 +176,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> {Acceleration, Distance, Gradient, Length, Miscellaneous, Number, ClassNumber, IdentityNumber, Qualifier, TimeDate, Speed, Text}</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="7"/>
@@ -208,13 +196,7 @@
     </r>
   </si>
   <si>
-    <t>{subset-26, subset-34}</t>
-  </si>
-  <si>
     <t xml:space="preserve">T_Definition </t>
-  </si>
-  <si>
-    <t>a textual and graphical description (all kind of picture, table and diagram are allowed)</t>
   </si>
   <si>
     <t>Files to complete this analysis</t>
@@ -414,6 +396,19 @@
   </si>
   <si>
     <t>Additional infomation to RBC</t>
+  </si>
+  <si>
+    <t>See embedded document</t>
+  </si>
+  <si>
+    <t>{3.3.0}</t>
+  </si>
+  <si>
+    <t>{subset-26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are the appropriate types and constants: 
+</t>
   </si>
 </sst>
 </file>
@@ -711,6 +706,10 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,10 +740,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1108,15 +1103,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1137,7 +1132,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
@@ -1172,7 +1167,7 @@
         <v>41591</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75">
@@ -1186,30 +1181,30 @@
     <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="16.5">
+    <row r="19" spans="1:5" ht="15.75">
       <c r="A19" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16.5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:5" ht="18.75">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="16.5">
+    <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75">
@@ -1224,13 +1219,13 @@
       <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="66.75" customHeight="1">
-      <c r="A28" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="A28" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="1"/>
@@ -1240,19 +1235,19 @@
     </row>
     <row r="31" spans="1:5" ht="18.75">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="19"/>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="20"/>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1281,7 @@
     <col min="10" max="10" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" thickBot="1">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1318,17 +1313,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31.5">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="A2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1343,18 +1338,18 @@
       <c r="H2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="25"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1367,249 +1362,249 @@
       <c r="H3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" ht="75">
-      <c r="A4" s="33" t="s">
-        <v>72</v>
+      <c r="A4" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="32">
+        <v>63</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="22">
         <v>1</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>70</v>
+      <c r="J4" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60">
-      <c r="A5" s="33"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="E5" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="E5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="33" t="s">
-        <v>73</v>
+      <c r="A6" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="32">
+        <v>63</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="22">
         <v>1</v>
       </c>
-      <c r="J6" s="32" t="s">
-        <v>82</v>
+      <c r="J6" s="22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="90">
-      <c r="A7" s="33"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
+      <c r="E7" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" ht="45">
-      <c r="A8" s="33" t="s">
-        <v>74</v>
+      <c r="A8" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="32">
+        <v>63</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="22">
         <v>1</v>
       </c>
-      <c r="J8" s="32" t="s">
-        <v>86</v>
+      <c r="J8" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90">
-      <c r="A9" s="33"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="E9" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" ht="45">
-      <c r="A10" s="33" t="s">
-        <v>75</v>
+      <c r="A10" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="32">
+        <v>63</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="22">
         <v>1</v>
       </c>
-      <c r="J10" s="32" t="s">
-        <v>90</v>
+      <c r="J10" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="33"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="E11" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="33"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="E12" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="33" t="s">
-        <v>76</v>
+      <c r="A13" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="32">
+        <v>63</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="22">
         <v>0</v>
       </c>
-      <c r="J13" s="32" t="s">
-        <v>95</v>
+      <c r="J13" s="22" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45">
-      <c r="A14" s="33" t="s">
-        <v>77</v>
+      <c r="A14" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="32">
+        <v>63</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="22">
         <v>0</v>
       </c>
-      <c r="J14" s="32" t="s">
-        <v>96</v>
+      <c r="J14" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45">
@@ -1617,15 +1612,15 @@
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="E15" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10">
@@ -1633,11 +1628,11 @@
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10">
@@ -1645,11 +1640,11 @@
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10">
@@ -1657,11 +1652,11 @@
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10">
@@ -1669,11 +1664,11 @@
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10">
@@ -1681,11 +1676,11 @@
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10">
@@ -1693,11 +1688,11 @@
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10">
@@ -1705,11 +1700,11 @@
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="14"/>
     </row>
   </sheetData>
@@ -1772,28 +1767,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -1801,31 +1796,31 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9">
@@ -2000,80 +1995,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="30" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2088,24 +2083,24 @@
       <c r="I3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
@@ -2118,9 +2113,9 @@
       <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="14"/>
@@ -2278,17 +2273,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="G1:G2"/>
@@ -2296,6 +2280,17 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2343,25 +2338,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -2369,29 +2364,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
@@ -2551,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2561,29 +2556,29 @@
     <col min="2" max="2" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="24" t="s">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="17" t="s">
@@ -2591,75 +2586,75 @@
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:5" ht="16.5">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="17"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="16.5">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="17"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="16.5">
+    <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.5">
-      <c r="A9" s="17" t="s">
+      <c r="B9" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.5">
-      <c r="A10" s="17" t="s">
+      <c r="B11" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B12" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="117" customHeight="1">
+      <c r="A13" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="63">
-      <c r="A11" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.5">
-      <c r="A12" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="47.25">
-      <c r="A13" s="17" t="s">
-        <v>52</v>
-      </c>
       <c r="B13" s="18" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="16.5">
+    <row r="14" spans="1:5">
       <c r="E14" s="3"/>
     </row>
   </sheetData>
@@ -2670,5 +2665,9 @@
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <oleObjects>
+    <oleObject progId="Dokument" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId2"/>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>